<commit_message>
added additional comments and reorganized files
</commit_message>
<xml_diff>
--- a/excel-sheets/averaged-arm-study-data2.xlsx
+++ b/excel-sheets/averaged-arm-study-data2.xlsx
@@ -440,7 +440,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -450,7 +450,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -460,7 +460,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -470,7 +470,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -480,7 +480,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -490,7 +490,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -500,7 +500,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -510,7 +510,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>5.666666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -520,7 +520,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>4.666666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -530,7 +530,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>4.833333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
@@ -540,7 +540,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -550,7 +550,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>4.833333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
@@ -560,7 +560,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>4.833333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
@@ -570,7 +570,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>5.333333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
@@ -580,7 +580,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>4.166666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
@@ -590,7 +590,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>3.333333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
@@ -600,7 +600,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>4.833333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
@@ -610,7 +610,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>3.166666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
@@ -620,7 +620,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>3.166666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
@@ -630,7 +630,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
@@ -640,7 +640,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>2.666666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23">
@@ -650,7 +650,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24">
@@ -660,7 +660,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
@@ -670,7 +670,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
@@ -680,7 +680,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
@@ -690,7 +690,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28">
@@ -700,7 +700,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29">
@@ -710,7 +710,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30">
@@ -720,7 +720,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>4.833333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31">
@@ -730,7 +730,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32">
@@ -740,7 +740,7 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>5.333333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
@@ -750,7 +750,7 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>5.666666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34">
@@ -760,7 +760,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>5.166666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35">
@@ -770,7 +770,7 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>5.666666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36">
@@ -780,7 +780,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37">
@@ -790,7 +790,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38">
@@ -800,7 +800,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>4.666666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39">
@@ -810,7 +810,7 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>5.333333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40">
@@ -820,7 +820,7 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>4.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41">
@@ -830,7 +830,7 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>2.666666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42">
@@ -840,7 +840,7 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>3.333333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43">
@@ -850,7 +850,7 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>3.166666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44">
@@ -860,7 +860,7 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45">
@@ -870,7 +870,7 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46">
@@ -880,7 +880,7 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47">
@@ -890,7 +890,7 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48">
@@ -900,7 +900,7 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49">
@@ -910,7 +910,7 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50">
@@ -920,7 +920,7 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51">
@@ -930,7 +930,7 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>4.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52">
@@ -940,7 +940,7 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>4.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53">
@@ -950,7 +950,7 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54">
@@ -960,7 +960,7 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>4.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55">
@@ -970,7 +970,7 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>5.166666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56">
@@ -980,7 +980,7 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>4.833333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57">
@@ -990,7 +990,7 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>5.333333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58">
@@ -1000,7 +1000,7 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59">
@@ -1010,7 +1010,7 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60">
@@ -1020,7 +1020,7 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>4.666666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61">
@@ -1030,7 +1030,7 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>2.833333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62">
@@ -1040,7 +1040,7 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>2.666666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63">
@@ -1050,7 +1050,7 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>3.333333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64">
@@ -1060,7 +1060,7 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>2.833333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65">
@@ -1070,7 +1070,7 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66">
@@ -1080,7 +1080,7 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67">
@@ -1090,7 +1090,7 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68">
@@ -1100,7 +1100,7 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69">
@@ -1110,7 +1110,7 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70">
@@ -1120,7 +1120,7 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71">
@@ -1130,7 +1130,7 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72">
@@ -1140,7 +1140,7 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>3.833333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73">
@@ -1150,7 +1150,7 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>4.666666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74">
@@ -1160,7 +1160,7 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>4.666666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75">
@@ -1170,7 +1170,7 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>4.333333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76">
@@ -1180,7 +1180,7 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>4.333333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77">
@@ -1190,7 +1190,7 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>3.166666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78">
@@ -1200,7 +1200,7 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>5.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79">
@@ -1210,7 +1210,7 @@
         </is>
       </c>
       <c r="B79" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80">
@@ -1220,7 +1220,7 @@
         </is>
       </c>
       <c r="B80" t="n">
-        <v>3.666666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81">
@@ -1230,7 +1230,7 @@
         </is>
       </c>
       <c r="B81" t="n">
-        <v>5.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82">
@@ -1240,7 +1240,7 @@
         </is>
       </c>
       <c r="B82" t="n">
-        <v>2.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83">
@@ -1250,7 +1250,7 @@
         </is>
       </c>
       <c r="B83" t="n">
-        <v>2.833333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84">
@@ -1260,7 +1260,7 @@
         </is>
       </c>
       <c r="B84" t="n">
-        <v>3.166666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85">
@@ -1270,7 +1270,7 @@
         </is>
       </c>
       <c r="B85" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86">
@@ -1280,7 +1280,7 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87">
@@ -1290,7 +1290,7 @@
         </is>
       </c>
       <c r="B87" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88">
@@ -1300,7 +1300,7 @@
         </is>
       </c>
       <c r="B88" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89">
@@ -1310,7 +1310,7 @@
         </is>
       </c>
       <c r="B89" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90">
@@ -1320,7 +1320,7 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91">
@@ -1330,7 +1330,7 @@
         </is>
       </c>
       <c r="B91" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92">
@@ -1340,7 +1340,7 @@
         </is>
       </c>
       <c r="B92" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93">
@@ -1350,7 +1350,7 @@
         </is>
       </c>
       <c r="B93" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94">
@@ -1360,7 +1360,7 @@
         </is>
       </c>
       <c r="B94" t="n">
-        <v>4.166666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95">
@@ -1370,7 +1370,7 @@
         </is>
       </c>
       <c r="B95" t="n">
-        <v>5.666666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96">
@@ -1380,7 +1380,7 @@
         </is>
       </c>
       <c r="B96" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97">
@@ -1390,7 +1390,7 @@
         </is>
       </c>
       <c r="B97" t="n">
-        <v>4.666666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98">
@@ -1400,7 +1400,7 @@
         </is>
       </c>
       <c r="B98" t="n">
-        <v>2.833333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99">
@@ -1410,7 +1410,7 @@
         </is>
       </c>
       <c r="B99" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100">
@@ -1420,7 +1420,7 @@
         </is>
       </c>
       <c r="B100" t="n">
-        <v>7.166666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="101">
@@ -1430,7 +1430,7 @@
         </is>
       </c>
       <c r="B101" t="n">
-        <v>3.666666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102">
@@ -1440,7 +1440,7 @@
         </is>
       </c>
       <c r="B102" t="n">
-        <v>4.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="103">
@@ -1450,7 +1450,7 @@
         </is>
       </c>
       <c r="B103" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="104">
@@ -1460,7 +1460,7 @@
         </is>
       </c>
       <c r="B104" t="n">
-        <v>2.833333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105">
@@ -1470,7 +1470,7 @@
         </is>
       </c>
       <c r="B105" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="106">
@@ -1480,7 +1480,7 @@
         </is>
       </c>
       <c r="B106" t="n">
-        <v>2.666666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="107">
@@ -1490,7 +1490,7 @@
         </is>
       </c>
       <c r="B107" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="108">
@@ -1500,7 +1500,7 @@
         </is>
       </c>
       <c r="B108" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="109">
@@ -1510,7 +1510,7 @@
         </is>
       </c>
       <c r="B109" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="110">
@@ -1520,7 +1520,7 @@
         </is>
       </c>
       <c r="B110" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="111">
@@ -1530,7 +1530,7 @@
         </is>
       </c>
       <c r="B111" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112">
@@ -1540,7 +1540,7 @@
         </is>
       </c>
       <c r="B112" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="113">
@@ -1550,7 +1550,7 @@
         </is>
       </c>
       <c r="B113" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="114">
@@ -1560,7 +1560,7 @@
         </is>
       </c>
       <c r="B114" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="115">
@@ -1570,7 +1570,7 @@
         </is>
       </c>
       <c r="B115" t="n">
-        <v>5.166666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="116">
@@ -1580,7 +1580,7 @@
         </is>
       </c>
       <c r="B116" t="n">
-        <v>5.333333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="117">
@@ -1590,7 +1590,7 @@
         </is>
       </c>
       <c r="B117" t="n">
-        <v>5.166666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="118">
@@ -1600,7 +1600,7 @@
         </is>
       </c>
       <c r="B118" t="n">
-        <v>4.333333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="119">
@@ -1610,7 +1610,7 @@
         </is>
       </c>
       <c r="B119" t="n">
-        <v>3.833333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="120">
@@ -1620,7 +1620,7 @@
         </is>
       </c>
       <c r="B120" t="n">
-        <v>5.833333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="121">
@@ -1630,7 +1630,7 @@
         </is>
       </c>
       <c r="B121" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="122">
@@ -1640,7 +1640,7 @@
         </is>
       </c>
       <c r="B122" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="123">
@@ -1650,7 +1650,7 @@
         </is>
       </c>
       <c r="B123" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="124">
@@ -1660,7 +1660,7 @@
         </is>
       </c>
       <c r="B124" t="n">
-        <v>3.166666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="125">
@@ -1670,7 +1670,7 @@
         </is>
       </c>
       <c r="B125" t="n">
-        <v>3.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="126">
@@ -1680,7 +1680,7 @@
         </is>
       </c>
       <c r="B126" t="n">
-        <v>2.666666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="127">
@@ -1690,7 +1690,7 @@
         </is>
       </c>
       <c r="B127" t="n">
-        <v>3.166666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="128">
@@ -1700,7 +1700,7 @@
         </is>
       </c>
       <c r="B128" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="129">
@@ -1710,7 +1710,7 @@
         </is>
       </c>
       <c r="B129" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="130">
@@ -1720,7 +1720,7 @@
         </is>
       </c>
       <c r="B130" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="131">
@@ -1730,7 +1730,7 @@
         </is>
       </c>
       <c r="B131" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132">
@@ -1740,7 +1740,7 @@
         </is>
       </c>
       <c r="B132" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="133">
@@ -1750,7 +1750,7 @@
         </is>
       </c>
       <c r="B133" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="134">
@@ -1760,7 +1760,7 @@
         </is>
       </c>
       <c r="B134" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="135">
@@ -1770,7 +1770,7 @@
         </is>
       </c>
       <c r="B135" t="n">
-        <v>5.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="136">
@@ -1780,7 +1780,7 @@
         </is>
       </c>
       <c r="B136" t="n">
-        <v>4.833333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="137">
@@ -1790,7 +1790,7 @@
         </is>
       </c>
       <c r="B137" t="n">
-        <v>6.666666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="138">
@@ -1800,7 +1800,7 @@
         </is>
       </c>
       <c r="B138" t="n">
-        <v>6.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="139">
@@ -1810,7 +1810,7 @@
         </is>
       </c>
       <c r="B139" t="n">
-        <v>6.166666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="140">
@@ -1820,7 +1820,7 @@
         </is>
       </c>
       <c r="B140" t="n">
-        <v>3.166666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="141">
@@ -1830,7 +1830,7 @@
         </is>
       </c>
       <c r="B141" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="142">
@@ -1840,7 +1840,7 @@
         </is>
       </c>
       <c r="B142" t="n">
-        <v>4.333333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="143">
@@ -1850,7 +1850,7 @@
         </is>
       </c>
       <c r="B143" t="n">
-        <v>3.333333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="144">
@@ -1860,7 +1860,7 @@
         </is>
       </c>
       <c r="B144" t="n">
-        <v>2.666666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="145">
@@ -1870,7 +1870,7 @@
         </is>
       </c>
       <c r="B145" t="n">
-        <v>2.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="146">
@@ -1880,7 +1880,7 @@
         </is>
       </c>
       <c r="B146" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="147">
@@ -1890,7 +1890,7 @@
         </is>
       </c>
       <c r="B147" t="n">
-        <v>1.833333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="148">
@@ -1900,7 +1900,7 @@
         </is>
       </c>
       <c r="B148" t="n">
-        <v>2.166666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="149">
@@ -1910,7 +1910,7 @@
         </is>
       </c>
       <c r="B149" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="150">
@@ -1920,7 +1920,7 @@
         </is>
       </c>
       <c r="B150" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="151">
@@ -1930,7 +1930,7 @@
         </is>
       </c>
       <c r="B151" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="152">
@@ -1940,7 +1940,7 @@
         </is>
       </c>
       <c r="B152" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="153">
@@ -1950,7 +1950,7 @@
         </is>
       </c>
       <c r="B153" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="154">
@@ -1960,7 +1960,7 @@
         </is>
       </c>
       <c r="B154" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="155">
@@ -1970,7 +1970,7 @@
         </is>
       </c>
       <c r="B155" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="156">
@@ -1980,7 +1980,7 @@
         </is>
       </c>
       <c r="B156" t="n">
-        <v>5.666666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="157">
@@ -1990,7 +1990,7 @@
         </is>
       </c>
       <c r="B157" t="n">
-        <v>4.166666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="158">
@@ -2000,7 +2000,7 @@
         </is>
       </c>
       <c r="B158" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="159">
@@ -2010,7 +2010,7 @@
         </is>
       </c>
       <c r="B159" t="n">
-        <v>6.833333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="160">
@@ -2020,7 +2020,7 @@
         </is>
       </c>
       <c r="B160" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="161">
@@ -2030,7 +2030,7 @@
         </is>
       </c>
       <c r="B161" t="n">
-        <v>3.666666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="162">
@@ -2040,7 +2040,7 @@
         </is>
       </c>
       <c r="B162" t="n">
-        <v>3.166666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="163">
@@ -2050,7 +2050,7 @@
         </is>
       </c>
       <c r="B163" t="n">
-        <v>5.333333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="164">
@@ -2060,7 +2060,7 @@
         </is>
       </c>
       <c r="B164" t="n">
-        <v>4.833333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="165">
@@ -2070,7 +2070,7 @@
         </is>
       </c>
       <c r="B165" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="166">
@@ -2080,7 +2080,7 @@
         </is>
       </c>
       <c r="B166" t="n">
-        <v>4.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="167">
@@ -2090,7 +2090,7 @@
         </is>
       </c>
       <c r="B167" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="168">
@@ -2100,7 +2100,7 @@
         </is>
       </c>
       <c r="B168" t="n">
-        <v>2.333333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="169">
@@ -2110,7 +2110,7 @@
         </is>
       </c>
       <c r="B169" t="n">
-        <v>1.833333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="170">
@@ -2120,7 +2120,7 @@
         </is>
       </c>
       <c r="B170" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="171">
@@ -2130,7 +2130,7 @@
         </is>
       </c>
       <c r="B171" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="172">
@@ -2140,7 +2140,7 @@
         </is>
       </c>
       <c r="B172" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="173">
@@ -2150,7 +2150,7 @@
         </is>
       </c>
       <c r="B173" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="174">
@@ -2160,7 +2160,7 @@
         </is>
       </c>
       <c r="B174" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="175">
@@ -2170,7 +2170,7 @@
         </is>
       </c>
       <c r="B175" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="176">
@@ -2180,7 +2180,7 @@
         </is>
       </c>
       <c r="B176" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="177">
@@ -2190,7 +2190,7 @@
         </is>
       </c>
       <c r="B177" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="178">
@@ -2200,7 +2200,7 @@
         </is>
       </c>
       <c r="B178" t="n">
-        <v>5.333333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="179">
@@ -2210,7 +2210,7 @@
         </is>
       </c>
       <c r="B179" t="n">
-        <v>6.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="180">
@@ -2220,7 +2220,7 @@
         </is>
       </c>
       <c r="B180" t="n">
-        <v>6.333333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="181">
@@ -2230,7 +2230,7 @@
         </is>
       </c>
       <c r="B181" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="182">
@@ -2240,7 +2240,7 @@
         </is>
       </c>
       <c r="B182" t="n">
-        <v>3.333333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="183">
@@ -2250,7 +2250,7 @@
         </is>
       </c>
       <c r="B183" t="n">
-        <v>3.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="184">
@@ -2260,7 +2260,7 @@
         </is>
       </c>
       <c r="B184" t="n">
-        <v>3.166666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="185">
@@ -2270,7 +2270,7 @@
         </is>
       </c>
       <c r="B185" t="n">
-        <v>4.666666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="186">
@@ -2280,7 +2280,7 @@
         </is>
       </c>
       <c r="B186" t="n">
-        <v>3.333333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="187">
@@ -2290,7 +2290,7 @@
         </is>
       </c>
       <c r="B187" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="188">
@@ -2300,7 +2300,7 @@
         </is>
       </c>
       <c r="B188" t="n">
-        <v>3.833333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="189">
@@ -2310,7 +2310,7 @@
         </is>
       </c>
       <c r="B189" t="n">
-        <v>2.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="190">
@@ -2320,7 +2320,7 @@
         </is>
       </c>
       <c r="B190" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>